<commit_message>
updates from Mike on 13Jun19
</commit_message>
<xml_diff>
--- a/LocationShots/TOCs/Redemap.xlsx
+++ b/LocationShots/TOCs/Redemap.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="2" r:id="rId1"/>
     <sheet name="Screenshot1-Aerial" sheetId="3" r:id="rId2"/>
+    <sheet name="new one" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="120">
   <si>
     <t>Level1</t>
   </si>
@@ -430,7 +431,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="27">
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -465,6 +466,27 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
       </font>
@@ -491,6 +513,15 @@
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -505,22 +536,37 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G108" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G108" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <tableColumns count="7">
-    <tableColumn id="6" name="By" dataDxfId="17"/>
-    <tableColumn id="7" name="Value" dataDxfId="16"/>
-    <tableColumn id="1" name="Level0" dataDxfId="15"/>
-    <tableColumn id="2" name="Level1" dataDxfId="14"/>
-    <tableColumn id="3" name="Level2" dataDxfId="13"/>
-    <tableColumn id="4" name="Level3" dataDxfId="12"/>
-    <tableColumn id="5" name="Ticked" dataDxfId="11"/>
+    <tableColumn id="6" name="By" dataDxfId="24"/>
+    <tableColumn id="7" name="Value" dataDxfId="23"/>
+    <tableColumn id="1" name="Level0" dataDxfId="22"/>
+    <tableColumn id="2" name="Level1" dataDxfId="21"/>
+    <tableColumn id="3" name="Level2" dataDxfId="20"/>
+    <tableColumn id="4" name="Level3" dataDxfId="19"/>
+    <tableColumn id="5" name="Ticked" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:G108" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:G108" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <tableColumns count="7">
+    <tableColumn id="6" name="By" dataDxfId="15"/>
+    <tableColumn id="7" name="Value" dataDxfId="14"/>
+    <tableColumn id="1" name="Level0" dataDxfId="13"/>
+    <tableColumn id="2" name="Level1" dataDxfId="12"/>
+    <tableColumn id="3" name="Level2" dataDxfId="11"/>
+    <tableColumn id="4" name="Level3" dataDxfId="10"/>
+    <tableColumn id="5" name="Ticked" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:G108" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <tableColumns count="7">
     <tableColumn id="6" name="By" dataDxfId="6"/>
     <tableColumn id="7" name="Value" dataDxfId="5"/>
@@ -823,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G108"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -1460,9 +1506,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1472,8 +1518,683 @@
   <dimension ref="A1:G108"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G108" sqref="G108"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="3" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E11" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E15" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E16" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E18" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E20" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C22" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D23" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E24" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E25" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E26" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E27" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E28" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E29" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E30" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E31" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E32" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D33" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E34" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E35" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E36" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F37" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F38" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E39" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F40" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F41" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E42" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F43" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F44" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F45" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E46" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D47" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E48" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F49" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F50" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F51" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E52" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F53" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F54" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F55" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F56" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E57" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F58" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F59" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F60" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F61" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F62" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D64" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="65" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E65" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="66" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E66" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="67" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D67" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="68" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D68" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="69" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E69" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="70" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E70" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="71" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D71" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="72" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D72" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="73" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E73" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E74" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="75" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D75" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="76" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D76" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E77" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="78" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E78" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="79" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D79" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="80" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D80" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="81" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E81" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="82" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F82" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="83" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F83" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="84" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F84" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="85" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E85" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="86" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F86" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="87" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F87" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="88" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F88" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="89" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F89" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="90" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F90" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="91" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F91" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="92" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F92" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="93" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E93" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="94" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F94" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="95" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F95" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="96" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F96" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E97" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F98" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F99" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F100" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E101" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F102" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F103" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E104" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E105" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F106" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F107" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G108" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G108"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1551,6 +2272,9 @@
       <c r="E5" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="G5" s="2" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E6" s="2" t="s">
@@ -1575,11 +2299,17 @@
       <c r="E8" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="G8" s="2" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E9" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="G9" s="2" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -1591,9 +2321,6 @@
       <c r="E10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="2" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E11" s="2" t="s">
@@ -1609,9 +2336,6 @@
       <c r="D13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="2" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -1634,7 +2358,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>110</v>
       </c>
@@ -1644,16 +2368,13 @@
       <c r="E17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G17" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E18" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>110</v>
       </c>
@@ -1664,12 +2385,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E20" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>110</v>
       </c>
@@ -1679,216 +2400,255 @@
       <c r="E21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G21" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C22" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D23" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E24" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E25" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E26" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E27" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E28" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E29" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E30" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E31" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E32" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D33" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E34" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E35" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E36" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F37" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="38" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="G37" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F38" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="39" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="G38" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E39" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F40" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="41" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="G40" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F41" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="42" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="G41" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E42" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F43" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="44" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="G43" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F44" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="45" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="G44" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F45" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="46" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="G45" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E46" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D47" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E48" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F49" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F50" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G50" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F51" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G51" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E52" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F53" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G53" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F54" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G54" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F55" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G55" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F56" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G56" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E57" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F58" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F59" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F60" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F61" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F62" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>110</v>
       </c>
@@ -1899,87 +2659,114 @@
         <v>64</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D64" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="65" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E65" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="66" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E66" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="67" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D67" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="68" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="G67" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D68" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="69" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E69" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="70" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="G69" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E70" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="71" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="G70" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D71" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="72" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="G71" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D72" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="73" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E73" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="74" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="G73" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E74" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="75" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="G74" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D75" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D76" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E77" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="78" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="G77" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E78" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="79" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="G78" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D79" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="80" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="G79" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D80" s="2" t="s">
         <v>80</v>
       </c>
@@ -2135,9 +2922,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding logging features for TOCScreenshot and TOCChoices
</commit_message>
<xml_diff>
--- a/LocationShots/TOCs/Redemap.xlsx
+++ b/LocationShots/TOCs/Redemap.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Template" sheetId="2" r:id="rId1"/>
     <sheet name="Screenshot1-Aerial" sheetId="3" r:id="rId2"/>
-    <sheet name="new one" sheetId="4" r:id="rId3"/>
+    <sheet name="Screenshot2" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -870,14 +870,16 @@
   <dimension ref="A1:G108"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="54.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.7109375" style="2" bestFit="1" customWidth="1"/>
@@ -1517,15 +1519,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="54.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.7109375" style="2" bestFit="1" customWidth="1"/>
@@ -2193,15 +2197,17 @@
   <dimension ref="A1:G108"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A63" sqref="A63"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C68" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="54.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36.85546875" style="2" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
reflect on the desired By object at runtime and exceute it
</commit_message>
<xml_diff>
--- a/LocationShots/TOCs/Redemap.xlsx
+++ b/LocationShots/TOCs/Redemap.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="126">
   <si>
     <t>Level1</t>
   </si>
@@ -210,9 +210,6 @@
     <t>Major Catchment Boundaries</t>
   </si>
   <si>
-    <t>City Plan Version 2</t>
-  </si>
-  <si>
     <t>Airport Environs Overlay</t>
   </si>
   <si>
@@ -376,6 +373,27 @@
   </si>
   <si>
     <t>chkBasemapVis</t>
+  </si>
+  <si>
+    <t>rbn_land</t>
+  </si>
+  <si>
+    <t>Land (RadioButton)</t>
+  </si>
+  <si>
+    <t>Land (CheckBox)</t>
+  </si>
+  <si>
+    <t>chkLayerVis_0</t>
+  </si>
+  <si>
+    <t>rbn_city_plan</t>
+  </si>
+  <si>
+    <t>City Plan Version 2 (CheckBox)</t>
+  </si>
+  <si>
+    <t>City Plan Version 2 (RadioButton)</t>
   </si>
 </sst>
 </file>
@@ -419,13 +437,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -536,7 +560,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G108" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G110" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <tableColumns count="7">
     <tableColumn id="6" name="By" dataDxfId="24"/>
     <tableColumn id="7" name="Value" dataDxfId="23"/>
@@ -551,7 +575,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:G108" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:G110" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <tableColumns count="7">
     <tableColumn id="6" name="By" dataDxfId="15"/>
     <tableColumn id="7" name="Value" dataDxfId="14"/>
@@ -566,7 +590,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:G108" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:G110" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <tableColumns count="7">
     <tableColumn id="6" name="By" dataDxfId="6"/>
     <tableColumn id="7" name="Value" dataDxfId="5"/>
@@ -867,33 +891,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G108"/>
+  <dimension ref="A1:G110"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="54.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" style="2" customWidth="1"/>
     <col min="8" max="16384" width="3" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>12</v>
@@ -913,624 +937,659 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>2</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E4" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E5" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E7" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B8" s="2" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E10" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E9" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E10" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E11" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E12" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D13" s="2" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D14" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E14" s="2" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E15" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E16" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B17" s="2" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B19" s="2" t="s">
+      <c r="E20" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E20" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E21" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C22" s="2" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C23" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D23" s="2" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D24" s="2" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E24" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E25" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E26" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E27" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E28" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E29" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E30" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E31" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E32" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E33" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D33" s="2" t="s">
+    <row r="34" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D34" s="2" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="34" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E34" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="35" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E35" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E36" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E37" s="2" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="37" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="F37" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="38" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F38" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F39" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E39" s="2" t="s">
+    <row r="40" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E40" s="2" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="40" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="F40" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="41" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F41" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F42" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E42" s="2" t="s">
+    <row r="43" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E43" s="2" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="43" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="F43" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="44" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F44" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F45" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F46" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E46" s="2" t="s">
+    <row r="47" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E47" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D47" s="2" t="s">
+    <row r="48" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D48" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E48" s="2" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E49" s="2" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F49" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F50" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F51" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F52" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E52" s="2" t="s">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E53" s="2" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F53" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F54" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F55" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F56" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F57" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E57" s="2" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E58" s="2" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F58" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F59" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F60" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F61" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F62" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F63" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C63" s="2" t="s">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D66" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D64" s="2" t="s">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E67" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="65" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E65" s="2" t="s">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E68" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="66" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E66" s="2" t="s">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D69" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="67" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D67" s="2" t="s">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D70" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="68" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D68" s="2" t="s">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E71" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="69" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E69" s="2" t="s">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E72" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="70" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E70" s="2" t="s">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D73" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="71" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D71" s="2" t="s">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D74" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E75" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="72" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D72" s="2" t="s">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E76" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D77" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="73" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E73" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="74" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E74" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="75" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D75" s="2" t="s">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D78" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D76" s="2" t="s">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E79" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E77" s="2" t="s">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E80" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E78" s="2" t="s">
+    <row r="81" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D81" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="79" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D79" s="2" t="s">
+    <row r="82" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D82" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="80" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D80" s="2" t="s">
+    <row r="83" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E83" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="81" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E81" s="2" t="s">
+    <row r="84" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F84" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="82" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F82" s="2" t="s">
+    <row r="85" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F85" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="83" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F83" s="2" t="s">
+    <row r="86" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F86" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="84" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F84" s="2" t="s">
+    <row r="87" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E87" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="85" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E85" s="2" t="s">
+    <row r="88" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F88" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="86" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F86" s="2" t="s">
+    <row r="89" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F89" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="87" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F87" s="2" t="s">
+    <row r="90" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F90" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="88" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F88" s="2" t="s">
+    <row r="91" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F91" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="89" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F89" s="2" t="s">
+    <row r="92" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F92" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="90" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F90" s="2" t="s">
+    <row r="93" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F93" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="91" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F91" s="2" t="s">
+    <row r="94" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F94" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="92" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F92" s="2" t="s">
+    <row r="95" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E95" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="93" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E93" s="2" t="s">
+    <row r="96" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F96" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="94" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F94" s="2" t="s">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F97" s="2" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="95" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F95" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="96" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F96" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E97" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F98" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F99" s="2" t="s">
-        <v>98</v>
+      <c r="E99" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F100" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E101" s="2" t="s">
-        <v>100</v>
+      <c r="F101" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F102" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E103" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F104" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F105" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F103" s="2" t="s">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E106" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E104" s="2" t="s">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E107" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E105" s="2" t="s">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F108" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F106" s="2" t="s">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F109" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C110" s="2" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F107" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G108"/>
+  <dimension ref="A1:G110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="54.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36.85546875" style="2" bestFit="1" customWidth="1"/>
@@ -1540,10 +1599,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>12</v>
@@ -1563,623 +1622,659 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
       <c r="G2" s="2" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E4" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E5" s="2" t="s">
-        <v>4</v>
+      <c r="G5" s="2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="2" t="b">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B8" s="2" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E10" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E9" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E10" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E11" s="2" t="s">
-        <v>10</v>
+      <c r="G11" s="2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E12" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D13" s="2" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E14" s="2" t="s">
+      <c r="G14" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E15" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E16" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E17" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B17" s="2" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E19" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E18" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B19" s="2" t="s">
+      <c r="E20" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E21" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E20" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E21" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G21" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="2" t="s">
+      <c r="G22" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C23" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D23" s="2" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D24" s="2" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E24" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E25" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E26" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E27" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E28" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E29" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E30" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E31" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E32" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E33" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D33" s="2" t="s">
+    <row r="34" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D34" s="2" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="34" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E34" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="35" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E35" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E36" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E37" s="2" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="37" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="F37" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="38" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F38" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F39" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E39" s="2" t="s">
+    <row r="40" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E40" s="2" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="40" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="F40" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="41" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F41" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F42" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E42" s="2" t="s">
+    <row r="43" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E43" s="2" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="43" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="F43" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="44" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F44" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F45" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F46" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E46" s="2" t="s">
+    <row r="47" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E47" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D47" s="2" t="s">
+    <row r="48" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D48" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E48" s="2" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E49" s="2" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F49" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F50" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F51" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F52" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E52" s="2" t="s">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E53" s="2" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F53" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F54" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F55" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F56" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F57" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E57" s="2" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E58" s="2" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F58" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F59" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F60" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F61" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F62" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F63" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C63" s="2" t="s">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D66" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D64" s="2" t="s">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E67" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="65" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E65" s="2" t="s">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E68" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="66" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E66" s="2" t="s">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D69" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="67" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D67" s="2" t="s">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D70" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="68" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D68" s="2" t="s">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E71" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="69" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E69" s="2" t="s">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E72" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="70" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E70" s="2" t="s">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D73" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="71" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D71" s="2" t="s">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D74" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E75" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="72" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D72" s="2" t="s">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E76" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D77" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="73" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E73" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="74" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E74" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="75" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D75" s="2" t="s">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D78" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D76" s="2" t="s">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E79" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E77" s="2" t="s">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E80" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E78" s="2" t="s">
+    <row r="81" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D81" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="79" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D79" s="2" t="s">
+    <row r="82" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D82" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="80" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D80" s="2" t="s">
+    <row r="83" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E83" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="81" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E81" s="2" t="s">
+    <row r="84" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F84" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="82" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F82" s="2" t="s">
+    <row r="85" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F85" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="83" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F83" s="2" t="s">
+    <row r="86" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F86" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="84" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F84" s="2" t="s">
+    <row r="87" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E87" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="85" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E85" s="2" t="s">
+    <row r="88" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F88" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="86" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F86" s="2" t="s">
+    <row r="89" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F89" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="87" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F87" s="2" t="s">
+    <row r="90" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F90" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="88" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F88" s="2" t="s">
+    <row r="91" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F91" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="89" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F89" s="2" t="s">
+    <row r="92" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F92" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="90" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F90" s="2" t="s">
+    <row r="93" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F93" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="91" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F91" s="2" t="s">
+    <row r="94" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F94" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="92" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F92" s="2" t="s">
+    <row r="95" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E95" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="93" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E93" s="2" t="s">
+    <row r="96" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F96" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="94" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F94" s="2" t="s">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F97" s="2" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="95" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F95" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="96" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F96" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E97" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F98" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F99" s="2" t="s">
-        <v>98</v>
+      <c r="E99" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F100" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E101" s="2" t="s">
-        <v>100</v>
+      <c r="F101" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F102" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E103" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F104" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F105" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F103" s="2" t="s">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E106" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E104" s="2" t="s">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E107" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E105" s="2" t="s">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F108" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F106" s="2" t="s">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F109" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C110" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F107" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G108" s="2" t="b">
+      <c r="G110" s="2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2194,33 +2289,33 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G108"/>
+  <dimension ref="A1:G110"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C68" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C74" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D96" sqref="D96"/>
+      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="54.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="3" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>12</v>
@@ -2240,43 +2335,60 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
       <c r="G2" s="2" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E4" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="G4" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E5" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="G5" s="2" t="b">
         <v>1</v>
@@ -2284,7 +2396,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G6" s="2" t="b">
         <v>1</v>
@@ -2292,249 +2404,249 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B8" s="2" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E10" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E11" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E12" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D13" s="2" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D14" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E14" s="2" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E15" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E16" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B17" s="2" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B19" s="2" t="s">
+      <c r="E20" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E20" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E21" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C22" s="2" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C23" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D23" s="2" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D24" s="2" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E24" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E25" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E26" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E27" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E28" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E29" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E30" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E31" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E32" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="E33" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D33" s="2" t="s">
+    <row r="34" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D34" s="2" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="34" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E34" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="35" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E35" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E36" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="E37" s="2" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="37" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="F37" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G37" s="2" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="38" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F38" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G38" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="F39" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G38" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E39" s="2" t="s">
+      <c r="G39" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="E40" s="2" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="40" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="F40" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G40" s="2" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="41" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F41" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G41" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="F42" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G41" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E42" s="2" t="s">
+      <c r="G42" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="E43" s="2" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="43" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="F43" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G43" s="2" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="44" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F44" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G44" s="2" t="b">
         <v>1</v>
@@ -2542,38 +2654,38 @@
     </row>
     <row r="45" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F45" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G45" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="F46" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G45" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E46" s="2" t="s">
+      <c r="G46" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="E47" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D47" s="2" t="s">
+    <row r="48" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D48" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E48" s="2" t="s">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E49" s="2" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F49" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G49" s="2" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F50" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G50" s="2" t="b">
         <v>1</v>
@@ -2581,28 +2693,28 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F51" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G51" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F52" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G51" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E52" s="2" t="s">
+      <c r="G52" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E53" s="2" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F53" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G53" s="2" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F54" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G54" s="2" t="b">
         <v>1</v>
@@ -2610,7 +2722,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F55" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G55" s="2" t="b">
         <v>1</v>
@@ -2618,311 +2730,330 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F56" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G56" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F57" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G56" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E57" s="2" t="s">
+      <c r="G57" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E58" s="2" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F58" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F59" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F60" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F61" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F62" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F63" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C63" s="2" t="s">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D66" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D64" s="2" t="s">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E67" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="65" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E65" s="2" t="s">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E68" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="66" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E66" s="2" t="s">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D69" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="67" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D67" s="2" t="s">
+      <c r="G69" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D70" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G67" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D68" s="2" t="s">
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E71" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="69" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E69" s="2" t="s">
+      <c r="G71" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E72" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="G69" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E70" s="2" t="s">
+      <c r="G72" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D73" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G70" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D71" s="2" t="s">
+      <c r="G73" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D74" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E75" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G71" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D72" s="2" t="s">
+      <c r="G75" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E76" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G76" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D77" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="73" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E73" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G73" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E74" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G74" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D75" s="2" t="s">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D78" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D76" s="2" t="s">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E79" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="77" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E77" s="2" t="s">
+      <c r="G79" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E80" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G77" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E78" s="2" t="s">
+      <c r="G80" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D81" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G78" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D79" s="2" t="s">
+      <c r="G81" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D82" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G79" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D80" s="2" t="s">
+    </row>
+    <row r="83" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="E83" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="81" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E81" s="2" t="s">
+    <row r="84" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="F84" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="82" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F82" s="2" t="s">
+    <row r="85" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="F85" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="83" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F83" s="2" t="s">
+    <row r="86" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="F86" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="84" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F84" s="2" t="s">
+    <row r="87" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="E87" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="85" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E85" s="2" t="s">
+    <row r="88" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="F88" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="86" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F86" s="2" t="s">
+    <row r="89" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="F89" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="87" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F87" s="2" t="s">
+    <row r="90" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="F90" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="88" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F88" s="2" t="s">
+    <row r="91" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="F91" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="89" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F89" s="2" t="s">
+    <row r="92" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="F92" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="90" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F90" s="2" t="s">
+    <row r="93" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="F93" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="91" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F91" s="2" t="s">
+    <row r="94" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="F94" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="92" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F92" s="2" t="s">
+    <row r="95" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="E95" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="93" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E93" s="2" t="s">
+    <row r="96" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="F96" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="94" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F94" s="2" t="s">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F97" s="2" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="95" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F95" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="96" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F96" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E97" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F98" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F99" s="2" t="s">
-        <v>98</v>
+      <c r="E99" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F100" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E101" s="2" t="s">
-        <v>100</v>
+      <c r="F101" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F102" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E103" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F104" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F105" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F103" s="2" t="s">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E106" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E104" s="2" t="s">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E107" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E105" s="2" t="s">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F108" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F106" s="2" t="s">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F109" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C110" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F107" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G108" s="2" t="b">
+      <c r="G110" s="2" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
more meaningful logging on the level of the screenshot
</commit_message>
<xml_diff>
--- a/LocationShots/TOCs/Redemap.xlsx
+++ b/LocationShots/TOCs/Redemap.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="2" r:id="rId1"/>
@@ -24,9 +24,6 @@
     <t>Level2</t>
   </si>
   <si>
-    <t>Land</t>
-  </si>
-  <si>
     <t>House - Unit Numbers</t>
   </si>
   <si>
@@ -394,6 +391,9 @@
   </si>
   <si>
     <t>City Plan Version 2 (RadioButton)</t>
+  </si>
+  <si>
+    <t>Land (Level1)</t>
   </si>
 </sst>
 </file>
@@ -893,11 +893,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C98" sqref="C98"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,13 +914,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -929,32 +929,32 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -962,14 +962,14 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>2</v>
+        <v>125</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -977,592 +977,592 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>110</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E6" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E7" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E8" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E10" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D14" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E16" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E17" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E19" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E21" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C23" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D24" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E25" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E26" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E27" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E28" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E29" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E30" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E31" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E32" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E33" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D34" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E35" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E36" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E37" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F38" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F39" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E40" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F41" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F42" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E43" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F44" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F45" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F46" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E47" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D48" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E49" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F50" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F51" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F52" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E53" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F54" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F55" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F56" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F57" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E58" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F59" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F60" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F61" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F62" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F63" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B64" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D66" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E67" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E68" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D69" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D70" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E71" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E72" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D73" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D74" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E75" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E76" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D77" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D78" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E79" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E80" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="81" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D81" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="82" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D82" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="83" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E83" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="84" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F84" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="85" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F85" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="86" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F86" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="87" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E87" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="88" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F88" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="89" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F89" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="90" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F90" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="91" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F91" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="92" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F92" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="93" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F93" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="94" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F94" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="95" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E95" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="96" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F96" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F97" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F98" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E99" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F100" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F101" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F102" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E103" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F104" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F105" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E106" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E107" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F108" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F109" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1582,7 +1582,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C65" sqref="C65"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1599,13 +1599,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -1614,21 +1614,21 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -1638,13 +1638,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -1654,14 +1654,14 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>2</v>
+        <v>125</v>
       </c>
       <c r="G4" s="2" t="b">
         <v>1</v>
@@ -1669,13 +1669,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>110</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G5" s="2" t="b">
         <v>1</v>
@@ -1683,12 +1683,12 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E6" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E7" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G7" s="2" t="b">
         <v>1</v>
@@ -1696,34 +1696,34 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E8" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E10" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G11" s="2" t="b">
         <v>1</v>
@@ -1731,17 +1731,17 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D14" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G14" s="2" t="b">
         <v>1</v>
@@ -1749,34 +1749,34 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E16" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E17" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G18" s="2" t="b">
         <v>1</v>
@@ -1784,34 +1784,34 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E19" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E21" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G22" s="2" t="b">
         <v>1</v>
@@ -1819,460 +1819,460 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C23" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D24" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E25" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E26" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E27" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E28" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E29" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E30" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E31" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E32" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E33" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D34" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E35" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E36" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E37" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F38" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F39" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E40" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F41" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F42" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E43" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F44" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F45" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F46" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E47" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D48" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E49" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F50" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F51" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F52" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E53" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F54" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F55" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F56" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F57" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E58" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F59" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F60" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F61" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F62" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F63" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B64" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D66" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E67" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E68" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D69" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D70" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E71" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E72" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D73" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D74" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E75" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E76" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D77" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D78" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E79" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E80" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="81" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D81" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="82" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D82" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="83" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E83" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="84" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F84" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="85" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F85" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="86" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F86" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="87" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E87" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="88" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F88" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="89" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F89" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="90" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F90" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="91" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F91" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="92" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F92" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="93" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F93" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="94" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F94" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="95" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E95" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="96" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F96" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F97" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F98" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E99" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F100" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F101" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F102" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E103" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F104" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F105" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E106" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E107" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F108" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F109" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G110" s="2" t="b">
         <v>1</v>
@@ -2291,11 +2291,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G110"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C74" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2312,13 +2312,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -2327,21 +2327,21 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -2351,13 +2351,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -2367,14 +2367,14 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>2</v>
+        <v>125</v>
       </c>
       <c r="G4" s="2" t="b">
         <v>1</v>
@@ -2382,13 +2382,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>110</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G5" s="2" t="b">
         <v>1</v>
@@ -2396,7 +2396,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E6" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G6" s="2" t="b">
         <v>1</v>
@@ -2404,7 +2404,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E7" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G7" s="2" t="b">
         <v>1</v>
@@ -2412,18 +2412,18 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E8" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G9" s="2" t="b">
         <v>1</v>
@@ -2431,7 +2431,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E10" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G10" s="2" t="b">
         <v>1</v>
@@ -2439,172 +2439,172 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D14" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E16" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E17" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E19" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E21" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C23" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D24" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E25" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E26" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E27" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E28" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E29" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E30" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E31" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E32" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E33" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D34" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E35" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E36" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E37" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F38" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G38" s="2" t="b">
         <v>1</v>
@@ -2612,7 +2612,7 @@
     </row>
     <row r="39" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F39" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G39" s="2" t="b">
         <v>1</v>
@@ -2620,12 +2620,12 @@
     </row>
     <row r="40" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E40" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F41" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G41" s="2" t="b">
         <v>1</v>
@@ -2633,7 +2633,7 @@
     </row>
     <row r="42" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F42" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G42" s="2" t="b">
         <v>1</v>
@@ -2641,12 +2641,12 @@
     </row>
     <row r="43" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E43" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F44" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G44" s="2" t="b">
         <v>1</v>
@@ -2654,7 +2654,7 @@
     </row>
     <row r="45" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F45" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G45" s="2" t="b">
         <v>1</v>
@@ -2662,7 +2662,7 @@
     </row>
     <row r="46" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F46" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G46" s="2" t="b">
         <v>1</v>
@@ -2670,22 +2670,22 @@
     </row>
     <row r="47" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E47" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D48" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E49" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F50" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G50" s="2" t="b">
         <v>1</v>
@@ -2693,7 +2693,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F51" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G51" s="2" t="b">
         <v>1</v>
@@ -2701,7 +2701,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F52" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G52" s="2" t="b">
         <v>1</v>
@@ -2709,12 +2709,12 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E53" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F54" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G54" s="2" t="b">
         <v>1</v>
@@ -2722,7 +2722,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F55" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G55" s="2" t="b">
         <v>1</v>
@@ -2730,7 +2730,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F56" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G56" s="2" t="b">
         <v>1</v>
@@ -2738,7 +2738,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F57" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G57" s="2" t="b">
         <v>1</v>
@@ -2746,74 +2746,74 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E58" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F59" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F60" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F61" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F62" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F63" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B64" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D66" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E67" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E68" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D69" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G69" s="2" t="b">
         <v>1</v>
@@ -2821,12 +2821,12 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D70" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E71" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G71" s="2" t="b">
         <v>1</v>
@@ -2834,7 +2834,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E72" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G72" s="2" t="b">
         <v>1</v>
@@ -2842,7 +2842,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D73" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G73" s="2" t="b">
         <v>1</v>
@@ -2850,12 +2850,12 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D74" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E75" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G75" s="2" t="b">
         <v>1</v>
@@ -2863,7 +2863,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E76" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G76" s="2" t="b">
         <v>1</v>
@@ -2871,17 +2871,17 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D77" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D78" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E79" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G79" s="2" t="b">
         <v>1</v>
@@ -2889,7 +2889,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E80" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G80" s="2" t="b">
         <v>1</v>
@@ -2897,7 +2897,7 @@
     </row>
     <row r="81" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D81" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G81" s="2" t="b">
         <v>1</v>
@@ -2905,153 +2905,153 @@
     </row>
     <row r="82" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D82" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="83" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E83" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="84" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F84" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="85" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F85" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="86" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F86" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="87" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E87" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="88" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F88" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="89" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F89" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="90" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F90" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="91" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F91" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="92" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F92" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="93" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F93" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="94" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F94" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="95" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E95" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="96" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F96" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F97" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F98" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E99" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F100" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F101" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F102" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E103" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F104" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F105" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E106" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E107" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F108" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F109" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G110" s="2" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
pressing TOC when it's invisible
</commit_message>
<xml_diff>
--- a/LocationShots/TOCs/Redemap.xlsx
+++ b/LocationShots/TOCs/Redemap.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="132">
   <si>
     <t>Level1</t>
   </si>
@@ -394,6 +394,24 @@
   </si>
   <si>
     <t>Land (Level1)</t>
+  </si>
+  <si>
+    <t>chkLayerVis_2</t>
+  </si>
+  <si>
+    <t>chkLayerVis_3</t>
+  </si>
+  <si>
+    <t>chkLayerVis_6</t>
+  </si>
+  <si>
+    <t>chkLayerVis_7</t>
+  </si>
+  <si>
+    <t>chkLayerVis_14</t>
+  </si>
+  <si>
+    <t>chkLayerVis_15</t>
   </si>
 </sst>
 </file>
@@ -457,22 +475,40 @@
   </cellStyles>
   <dxfs count="27">
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -496,16 +532,16 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -514,24 +550,6 @@
       <font>
         <b/>
       </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -563,45 +581,45 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G110" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="A1:G110"/>
   <tableColumns count="7">
-    <tableColumn id="6" name="By" dataDxfId="24"/>
-    <tableColumn id="7" name="Value" dataDxfId="23"/>
-    <tableColumn id="1" name="Level0" dataDxfId="22"/>
-    <tableColumn id="2" name="Level1" dataDxfId="21"/>
-    <tableColumn id="3" name="Level2" dataDxfId="20"/>
-    <tableColumn id="4" name="Level3" dataDxfId="19"/>
-    <tableColumn id="5" name="Ticked" dataDxfId="18"/>
+    <tableColumn id="6" name="By" dataDxfId="11"/>
+    <tableColumn id="7" name="Value" dataDxfId="10"/>
+    <tableColumn id="1" name="Level0" dataDxfId="9"/>
+    <tableColumn id="2" name="Level1" dataDxfId="8"/>
+    <tableColumn id="3" name="Level2" dataDxfId="7"/>
+    <tableColumn id="4" name="Level3" dataDxfId="6"/>
+    <tableColumn id="5" name="Ticked" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:G110" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:G110" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="A1:G110"/>
   <tableColumns count="7">
-    <tableColumn id="6" name="By" dataDxfId="15"/>
-    <tableColumn id="7" name="Value" dataDxfId="14"/>
-    <tableColumn id="1" name="Level0" dataDxfId="13"/>
-    <tableColumn id="2" name="Level1" dataDxfId="12"/>
-    <tableColumn id="3" name="Level2" dataDxfId="11"/>
-    <tableColumn id="4" name="Level3" dataDxfId="10"/>
-    <tableColumn id="5" name="Ticked" dataDxfId="9"/>
+    <tableColumn id="6" name="By" dataDxfId="21"/>
+    <tableColumn id="7" name="Value" dataDxfId="20"/>
+    <tableColumn id="1" name="Level0" dataDxfId="19"/>
+    <tableColumn id="2" name="Level1" dataDxfId="18"/>
+    <tableColumn id="3" name="Level2" dataDxfId="17"/>
+    <tableColumn id="4" name="Level3" dataDxfId="16"/>
+    <tableColumn id="5" name="Ticked" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:G110" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:G110" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A1:G110"/>
   <tableColumns count="7">
-    <tableColumn id="6" name="By" dataDxfId="6"/>
-    <tableColumn id="7" name="Value" dataDxfId="5"/>
-    <tableColumn id="1" name="Level0" dataDxfId="4"/>
-    <tableColumn id="2" name="Level1" dataDxfId="3"/>
-    <tableColumn id="3" name="Level2" dataDxfId="2"/>
-    <tableColumn id="4" name="Level3" dataDxfId="1"/>
-    <tableColumn id="5" name="Ticked" dataDxfId="0"/>
+    <tableColumn id="6" name="By" dataDxfId="5"/>
+    <tableColumn id="7" name="Value" dataDxfId="4"/>
+    <tableColumn id="1" name="Level0" dataDxfId="3"/>
+    <tableColumn id="2" name="Level1" dataDxfId="2"/>
+    <tableColumn id="3" name="Level2" dataDxfId="1"/>
+    <tableColumn id="4" name="Level3" dataDxfId="0"/>
+    <tableColumn id="5" name="Ticked" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -896,22 +914,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G110"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E40" sqref="E40"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:F110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="57.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="3" style="2"/>
   </cols>
   <sheetData>
@@ -948,6 +966,8 @@
       <c r="C2" s="2" t="s">
         <v>120</v>
       </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -959,8 +979,8 @@
       <c r="C3" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -974,8 +994,6 @@
       <c r="D4" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -990,11 +1008,23 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>126</v>
+      </c>
       <c r="E6" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="E7" s="2" t="s">
         <v>4</v>
       </c>
@@ -1016,6 +1046,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>128</v>
+      </c>
       <c r="E10" s="2" t="s">
         <v>7</v>
       </c>
@@ -1353,6 +1389,12 @@
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="D69" s="2" t="s">
         <v>66</v>
       </c>
@@ -1363,16 +1405,34 @@
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="E71" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>128</v>
+      </c>
       <c r="E72" s="2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>129</v>
+      </c>
       <c r="D73" s="2" t="s">
         <v>70</v>
       </c>
@@ -1403,91 +1463,109 @@
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="E79" s="2" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>130</v>
+      </c>
       <c r="E80" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="81" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>131</v>
+      </c>
       <c r="D81" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="82" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D82" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="83" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E83" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="84" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F84" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="85" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F85" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="86" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F86" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="87" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E87" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="88" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F88" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="89" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F89" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="90" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F90" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="91" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F91" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="92" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F92" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="93" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F93" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="94" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F94" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="95" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E95" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="96" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F96" s="2" t="s">
         <v>92</v>
       </c>
@@ -1581,22 +1659,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:F110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="57.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="3" style="2"/>
   </cols>
   <sheetData>
@@ -1685,11 +1763,23 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>126</v>
+      </c>
       <c r="E6" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="E7" s="2" t="s">
         <v>4</v>
       </c>
@@ -1714,6 +1804,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>128</v>
+      </c>
       <c r="E10" s="2" t="s">
         <v>7</v>
       </c>
@@ -2063,6 +2159,12 @@
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="D69" s="2" t="s">
         <v>66</v>
       </c>
@@ -2073,16 +2175,34 @@
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="E71" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>128</v>
+      </c>
       <c r="E72" s="2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>129</v>
+      </c>
       <c r="D73" s="2" t="s">
         <v>70</v>
       </c>
@@ -2113,91 +2233,109 @@
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="E79" s="2" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>130</v>
+      </c>
       <c r="E80" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="81" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>131</v>
+      </c>
       <c r="D81" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="82" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D82" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="83" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E83" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="84" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F84" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="85" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F85" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="86" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F86" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="87" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E87" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="88" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F88" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="89" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F89" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="90" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F90" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="91" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F91" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="92" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F92" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="93" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F93" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="94" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F94" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="95" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E95" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="96" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F96" s="2" t="s">
         <v>92</v>
       </c>
@@ -2295,21 +2433,21 @@
   <dimension ref="A1:G110"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E83" sqref="E83"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:F110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="3" style="2"/>
   </cols>
   <sheetData>
@@ -2398,6 +2536,12 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>126</v>
+      </c>
       <c r="E6" s="2" t="s">
         <v>3</v>
       </c>
@@ -2406,6 +2550,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="E7" s="2" t="s">
         <v>4</v>
       </c>
@@ -2433,6 +2583,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>128</v>
+      </c>
       <c r="E10" s="2" t="s">
         <v>7</v>
       </c>
@@ -2815,6 +2971,12 @@
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="D69" s="2" t="s">
         <v>66</v>
       </c>
@@ -2828,6 +2990,12 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="E71" s="2" t="s">
         <v>68</v>
       </c>
@@ -2836,6 +3004,12 @@
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>128</v>
+      </c>
       <c r="E72" s="2" t="s">
         <v>69</v>
       </c>
@@ -2844,6 +3018,12 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>129</v>
+      </c>
       <c r="D73" s="2" t="s">
         <v>70</v>
       </c>
@@ -2883,6 +3063,12 @@
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="E79" s="2" t="s">
         <v>75</v>
       </c>
@@ -2891,6 +3077,12 @@
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>130</v>
+      </c>
       <c r="E80" s="2" t="s">
         <v>76</v>
       </c>
@@ -2898,7 +3090,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>131</v>
+      </c>
       <c r="D81" s="2" t="s">
         <v>77</v>
       </c>
@@ -2906,77 +3104,77 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D82" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="83" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E83" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="84" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F84" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="85" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F85" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="86" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F86" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="87" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E87" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="88" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F88" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="89" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F89" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="90" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F90" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="91" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F91" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="92" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F92" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="93" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F93" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="94" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F94" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="95" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E95" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="96" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F96" s="2" t="s">
         <v>92</v>
       </c>
@@ -3062,9 +3260,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>